<commit_message>
Alterações realizadas nos códigos do IPEA para a dissertação
</commit_message>
<xml_diff>
--- a/output/regression_output/regression_table_1.xlsx
+++ b/output/regression_output/regression_table_1.xlsx
@@ -12,18 +12,165 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="145">
+  <si>
+    <t/>
+  </si>
   <si>
     <t>model</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
     <t>Dependent Var.:</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>(Intercept)</t>
+    <t>Constant</t>
   </si>
   <si>
     <t>f_compact_contig_inter_dens</t>
@@ -355,389 +502,536 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>54</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>56</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="C13" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>62</v>
+      </c>
+      <c r="C14" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="C15" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="C17" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>66</v>
+        <v>68</v>
+      </c>
+      <c r="C20" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>68</v>
+        <v>70</v>
+      </c>
+      <c r="C22" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>71</v>
+      </c>
+      <c r="C23" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="C24" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>73</v>
+      </c>
+      <c r="C25" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>75</v>
+      </c>
+      <c r="C27" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>74</v>
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="C29" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="C30" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="C31" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>80</v>
+      </c>
+      <c r="C32" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>82</v>
+      </c>
+      <c r="C34" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>83</v>
+      </c>
+      <c r="C35" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
+        <v>84</v>
+      </c>
+      <c r="C36" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>85</v>
+      </c>
+      <c r="C37" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="C38" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>87</v>
+      </c>
+      <c r="C39" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>86</v>
+        <v>88</v>
+      </c>
+      <c r="C40" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>90</v>
+      </c>
+      <c r="C42" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>89</v>
+        <v>91</v>
+      </c>
+      <c r="C43" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>92</v>
+      </c>
+      <c r="C44" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>91</v>
+        <v>93</v>
+      </c>
+      <c r="C45" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>92</v>
+        <v>94</v>
+      </c>
+      <c r="C46" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>93</v>
+        <v>95</v>
+      </c>
+      <c r="C47" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="C48" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>97</v>
+      </c>
+      <c r="C49" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>